<commit_message>
update data read and data out
</commit_message>
<xml_diff>
--- a/data/other.xlsx
+++ b/data/other.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubs\Dropbox (MIT)\Research\FDA1\data integration\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adubs\Documents\GitHub\glyc-hardware-int\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872BFD28-4473-40FD-B1BB-DA4C2C3D16DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2BCE61-EF3B-485F-B9C1-9666A92FE608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27396" yWindow="3060" windowWidth="13392" windowHeight="8076" xr2:uid="{248E64A1-F061-4A90-A392-C819CBD819BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{248E64A1-F061-4A90-A392-C819CBD819BC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,23 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Measurement</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Galactose</t>
   </si>
   <si>
-    <t>mM</t>
-  </si>
-  <si>
     <t>Uridine</t>
   </si>
   <si>
@@ -62,75 +50,24 @@
     <t>mAb</t>
   </si>
   <si>
-    <t>mg/L</t>
-  </si>
-  <si>
-    <t>AvgLive Diameter</t>
-  </si>
-  <si>
-    <t>TotalDensity</t>
-  </si>
-  <si>
     <t>Viability</t>
   </si>
   <si>
     <t>ViableDensity</t>
   </si>
   <si>
-    <t>Ca</t>
-  </si>
-  <si>
     <t>Gln</t>
   </si>
   <si>
-    <t>Glu</t>
-  </si>
-  <si>
     <t>Gluc</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Lac</t>
   </si>
   <si>
     <t>NH4</t>
   </si>
   <si>
-    <t>Osmo</t>
-  </si>
-  <si>
-    <t>pCO2</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>pO2</t>
-  </si>
-  <si>
-    <t>um</t>
-  </si>
-  <si>
-    <t>e5 cells/mL</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>g/L</t>
-  </si>
-  <si>
-    <t>mOsm/kg</t>
-  </si>
-  <si>
-    <t>mmHg</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
     <t>UDP-GlcNAc</t>
   </si>
   <si>
@@ -159,6 +96,18 @@
   </si>
   <si>
     <t>UDP-Glc</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>DL-Asparagine (Asn)</t>
+  </si>
+  <si>
+    <t>DL-Aspartic acid (Asp)</t>
   </si>
 </sst>
 </file>
@@ -174,12 +123,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Helvetica"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -538,265 +486,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811CA2B2-4519-4CB1-9AC5-6378F6E056CA}">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1E2B49-B2A5-4EC2-8B87-395A1AB49BF5}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.86328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>45530.5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4</v>
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>